<commit_message>
Add XLSX file and convert lens to JSON, created by GitHub Action
</commit_message>
<xml_diff>
--- a/custom-lens/cloud-foundations-accelerator-workbook.xlsx
+++ b/custom-lens/cloud-foundations-accelerator-workbook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="586">
   <si>
     <t>Cloud Foundations Accelerator Workbook</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Notes and Decisions</t>
   </si>
   <si>
-    <t>Create management account</t>
+    <t>Create AWS management account</t>
   </si>
   <si>
     <t>Configure management account</t>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Set up management account email address</t>
-  </si>
-  <si>
-    <t>Create AWS management account</t>
   </si>
   <si>
     <t>Secure management account root user</t>
@@ -2328,506 +2325,506 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2836,10 +2833,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2950,463 +2947,463 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3419,10 +3416,10 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3545,39 +3542,39 @@
         <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3588,13 +3585,13 @@
         <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3605,55 +3602,55 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3721,126 +3718,126 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3917,244 +3914,244 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4163,10 +4160,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4251,213 +4248,213 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4539,293 +4536,293 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4834,10 +4831,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4933,155 +4930,155 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5157,259 +5154,259 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5500,191 +5497,191 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:7">

</xml_diff>